<commit_message>
Univariate corrected. Multivariate needs changes.
</commit_message>
<xml_diff>
--- a/multivariate/data/processed/gdp_factor_india.xlsx
+++ b/multivariate/data/processed/gdp_factor_india.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,62 +446,37 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Official exchange rate (LCU per US$, period average)</t>
+          <t>Exports of goods and services (% of GDP)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Exports of goods and services (% of GDP)</t>
+          <t>GDP (current US$)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>GDP (current US$)</t>
+          <t>Final consumption expenditure (% of GDP)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>General government final consumption expenditure (% of GDP)</t>
+          <t>Imports of goods and services (% of GDP)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Final consumption expenditure (% of GDP)</t>
+          <t>Industry (including construction), value added (% of GDP)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Imports of goods and services (% of GDP)</t>
+          <t>Inflation, consumer prices (annual %)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Industry (including construction), value added (% of GDP)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Inflation, consumer prices (annual %)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Lending interest rate (%)</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
           <t>Gross capital formation (% of GDP)</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Broad money (% of GDP)</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Unemployment, total (% of total labor force) (modeled ILO estimate)</t>
         </is>
       </c>
     </row>
@@ -515,40 +490,25 @@
         <v>-1.58891131223691</v>
       </c>
       <c r="C2" t="n">
-        <v>22.7424333333333</v>
+        <v>8.49424077053547</v>
       </c>
       <c r="D2" t="n">
-        <v>8.49424077053547</v>
+        <v>270.105341879226</v>
       </c>
       <c r="E2" t="n">
-        <v>270.105341879226</v>
+        <v>78.0968001480887</v>
       </c>
       <c r="F2" t="n">
-        <v>11.0787262464783</v>
+        <v>8.49348578059959</v>
       </c>
       <c r="G2" t="n">
-        <v>78.0968001480887</v>
+        <v>26.4417201769254</v>
       </c>
       <c r="H2" t="n">
-        <v>8.49348578059959</v>
+        <v>13.8702461773683</v>
       </c>
       <c r="I2" t="n">
-        <v>26.4417201769254</v>
-      </c>
-      <c r="J2" t="n">
-        <v>13.8702461773683</v>
-      </c>
-      <c r="K2" t="n">
-        <v>17.875</v>
-      </c>
-      <c r="L2" t="n">
         <v>25.1405052782292</v>
-      </c>
-      <c r="M2" t="n">
-        <v>43.4178555336728</v>
-      </c>
-      <c r="N2" t="n">
-        <v>7.722</v>
       </c>
     </row>
     <row r="3">
@@ -561,40 +521,25 @@
         <v>-1.55624498023457</v>
       </c>
       <c r="C3" t="n">
-        <v>25.9180833333333</v>
+        <v>8.84292692502088</v>
       </c>
       <c r="D3" t="n">
-        <v>8.84292692502088</v>
+        <v>288.208070278013</v>
       </c>
       <c r="E3" t="n">
-        <v>288.208070278013</v>
+        <v>76.6593851383476</v>
       </c>
       <c r="F3" t="n">
-        <v>10.9150464795678</v>
+        <v>9.590172116807169</v>
       </c>
       <c r="G3" t="n">
-        <v>76.6593851383476</v>
+        <v>26.7927432696344</v>
       </c>
       <c r="H3" t="n">
-        <v>9.590172116807169</v>
+        <v>11.7878170418134</v>
       </c>
       <c r="I3" t="n">
-        <v>26.7927432696344</v>
-      </c>
-      <c r="J3" t="n">
-        <v>11.7878170418134</v>
-      </c>
-      <c r="K3" t="n">
-        <v>18.9166666666667</v>
-      </c>
-      <c r="L3" t="n">
         <v>27.44020415513</v>
-      </c>
-      <c r="M3" t="n">
-        <v>44.1444293103205</v>
-      </c>
-      <c r="N3" t="n">
-        <v>7.733</v>
       </c>
     </row>
     <row r="4">
@@ -607,40 +552,25 @@
         <v>-0.671618869530872</v>
       </c>
       <c r="C4" t="n">
-        <v>30.4932916666667</v>
+        <v>9.834217454863261</v>
       </c>
       <c r="D4" t="n">
-        <v>9.834217454863261</v>
+        <v>279.295648982529</v>
       </c>
       <c r="E4" t="n">
-        <v>279.295648982529</v>
+        <v>76.4542220201817</v>
       </c>
       <c r="F4" t="n">
-        <v>11.0026650353957</v>
+        <v>9.81732233160511</v>
       </c>
       <c r="G4" t="n">
-        <v>76.4542220201817</v>
+        <v>26.7815542820739</v>
       </c>
       <c r="H4" t="n">
-        <v>9.81732233160511</v>
+        <v>6.32689048779867</v>
       </c>
       <c r="I4" t="n">
-        <v>26.7815542820739</v>
-      </c>
-      <c r="J4" t="n">
-        <v>6.32689048779867</v>
-      </c>
-      <c r="K4" t="n">
-        <v>16.25</v>
-      </c>
-      <c r="L4" t="n">
         <v>22.716410511618</v>
-      </c>
-      <c r="M4" t="n">
-        <v>44.8834588757366</v>
-      </c>
-      <c r="N4" t="n">
-        <v>7.75</v>
       </c>
     </row>
     <row r="5">
@@ -653,40 +583,25 @@
         <v>-0.512193818555587</v>
       </c>
       <c r="C5" t="n">
-        <v>31.3737425</v>
+        <v>9.888084916445401</v>
       </c>
       <c r="D5" t="n">
-        <v>9.888084916445401</v>
+        <v>327.274843459429</v>
       </c>
       <c r="E5" t="n">
-        <v>327.274843459429</v>
+        <v>75.2766533814778</v>
       </c>
       <c r="F5" t="n">
-        <v>10.43581347191</v>
+        <v>10.1900594604801</v>
       </c>
       <c r="G5" t="n">
-        <v>75.2766533814778</v>
+        <v>27.6282012473106</v>
       </c>
       <c r="H5" t="n">
-        <v>10.1900594604801</v>
+        <v>10.2479355556119</v>
       </c>
       <c r="I5" t="n">
-        <v>27.6282012473106</v>
-      </c>
-      <c r="J5" t="n">
-        <v>10.2479355556119</v>
-      </c>
-      <c r="K5" t="n">
-        <v>14.75</v>
-      </c>
-      <c r="L5" t="n">
         <v>26.3101665553988</v>
-      </c>
-      <c r="M5" t="n">
-        <v>46.0214654858897</v>
-      </c>
-      <c r="N5" t="n">
-        <v>7.645</v>
       </c>
     </row>
     <row r="6">
@@ -699,40 +614,25 @@
         <v>-1.54413181166043</v>
       </c>
       <c r="C6" t="n">
-        <v>32.4270766666667</v>
+        <v>10.8439680350622</v>
       </c>
       <c r="D6" t="n">
-        <v>10.8439680350622</v>
+        <v>360.281909643489</v>
       </c>
       <c r="E6" t="n">
-        <v>360.281909643489</v>
+        <v>74.2407283976666</v>
       </c>
       <c r="F6" t="n">
-        <v>10.5402675188309</v>
+        <v>12.0234806711877</v>
       </c>
       <c r="G6" t="n">
-        <v>74.2407283976666</v>
+        <v>28.5998094242024</v>
       </c>
       <c r="H6" t="n">
-        <v>12.0234806711877</v>
+        <v>10.2248861637544</v>
       </c>
       <c r="I6" t="n">
-        <v>28.5998094242024</v>
-      </c>
-      <c r="J6" t="n">
-        <v>10.2248861637544</v>
-      </c>
-      <c r="K6" t="n">
-        <v>15.4583333333333</v>
-      </c>
-      <c r="L6" t="n">
         <v>29.1523371515588</v>
-      </c>
-      <c r="M6" t="n">
-        <v>43.545308881586</v>
-      </c>
-      <c r="N6" t="n">
-        <v>7.608</v>
       </c>
     </row>
     <row r="7">
@@ -745,40 +645,25 @@
         <v>-1.51595497295368</v>
       </c>
       <c r="C7" t="n">
-        <v>35.4331733333333</v>
+        <v>10.3851692716063</v>
       </c>
       <c r="D7" t="n">
-        <v>10.3851692716063</v>
+        <v>392.896866204516</v>
       </c>
       <c r="E7" t="n">
-        <v>392.896866204516</v>
+        <v>74.8861078483603</v>
       </c>
       <c r="F7" t="n">
-        <v>10.3308896774711</v>
+        <v>11.5443185997804</v>
       </c>
       <c r="G7" t="n">
-        <v>74.8861078483603</v>
+        <v>27.9122703698412</v>
       </c>
       <c r="H7" t="n">
-        <v>11.5443185997804</v>
+        <v>8.97715233826453</v>
       </c>
       <c r="I7" t="n">
-        <v>27.9122703698412</v>
-      </c>
-      <c r="J7" t="n">
-        <v>8.97715233826453</v>
-      </c>
-      <c r="K7" t="n">
-        <v>15.9583333333333</v>
-      </c>
-      <c r="L7" t="n">
         <v>22.7592531809279</v>
-      </c>
-      <c r="M7" t="n">
-        <v>44.6894365497978</v>
-      </c>
-      <c r="N7" t="n">
-        <v>7.558</v>
       </c>
     </row>
     <row r="8">
@@ -791,40 +676,25 @@
         <v>-0.713014326393888</v>
       </c>
       <c r="C8" t="n">
-        <v>36.3132858333333</v>
+        <v>10.690717318379</v>
       </c>
       <c r="D8" t="n">
-        <v>10.690717318379</v>
+        <v>415.867563592829</v>
       </c>
       <c r="E8" t="n">
-        <v>415.867563592829</v>
+        <v>74.94055852647929</v>
       </c>
       <c r="F8" t="n">
-        <v>11.0287262034071</v>
+        <v>11.9286695486689</v>
       </c>
       <c r="G8" t="n">
-        <v>74.94055852647929</v>
+        <v>27.8370307633106</v>
       </c>
       <c r="H8" t="n">
-        <v>11.9286695486689</v>
+        <v>7.16425211462724</v>
       </c>
       <c r="I8" t="n">
-        <v>27.8370307633106</v>
-      </c>
-      <c r="J8" t="n">
-        <v>7.16425211462724</v>
-      </c>
-      <c r="K8" t="n">
-        <v>13.8333333333333</v>
-      </c>
-      <c r="L8" t="n">
         <v>25.6927329065132</v>
-      </c>
-      <c r="M8" t="n">
-        <v>47.4599823040339</v>
-      </c>
-      <c r="N8" t="n">
-        <v>7.61</v>
       </c>
     </row>
     <row r="9">
@@ -837,40 +707,25 @@
         <v>-1.63832533358649</v>
       </c>
       <c r="C9" t="n">
-        <v>41.259365</v>
+        <v>11.0184691793102</v>
       </c>
       <c r="D9" t="n">
-        <v>11.0184691793102</v>
+        <v>421.351317224941</v>
       </c>
       <c r="E9" t="n">
-        <v>421.351317224941</v>
+        <v>75.7186237600651</v>
       </c>
       <c r="F9" t="n">
-        <v>11.9098898139839</v>
+        <v>12.6810008997545</v>
       </c>
       <c r="G9" t="n">
-        <v>75.7186237600651</v>
+        <v>27.3030378517565</v>
       </c>
       <c r="H9" t="n">
-        <v>12.6810008997545</v>
+        <v>13.2308389767977</v>
       </c>
       <c r="I9" t="n">
-        <v>27.3030378517565</v>
-      </c>
-      <c r="J9" t="n">
-        <v>13.2308389767977</v>
-      </c>
-      <c r="K9" t="n">
-        <v>13.5416666666667</v>
-      </c>
-      <c r="L9" t="n">
         <v>24.9753699423901</v>
-      </c>
-      <c r="M9" t="n">
-        <v>48.9013068508578</v>
-      </c>
-      <c r="N9" t="n">
-        <v>7.639</v>
       </c>
     </row>
     <row r="10">
@@ -883,40 +738,25 @@
         <v>-0.703547232193242</v>
       </c>
       <c r="C10" t="n">
-        <v>43.0554283333334</v>
+        <v>11.4520646128009</v>
       </c>
       <c r="D10" t="n">
-        <v>11.4520646128009</v>
+        <v>458.82105261579</v>
       </c>
       <c r="E10" t="n">
-        <v>458.82105261579</v>
+        <v>76.184976149322</v>
       </c>
       <c r="F10" t="n">
-        <v>12.1754896050679</v>
+        <v>13.363533431492</v>
       </c>
       <c r="G10" t="n">
-        <v>76.184976149322</v>
+        <v>26.5192933488596</v>
       </c>
       <c r="H10" t="n">
-        <v>13.363533431492</v>
+        <v>4.66982038037594</v>
       </c>
       <c r="I10" t="n">
-        <v>26.5192933488596</v>
-      </c>
-      <c r="J10" t="n">
-        <v>4.66982038037594</v>
-      </c>
-      <c r="K10" t="n">
-        <v>12.5416666666667</v>
-      </c>
-      <c r="L10" t="n">
         <v>30.9580879683861</v>
-      </c>
-      <c r="M10" t="n">
-        <v>51.0649259553469</v>
-      </c>
-      <c r="N10" t="n">
-        <v>7.617</v>
       </c>
     </row>
     <row r="11">
@@ -929,40 +769,25 @@
         <v>-0.982342580017138</v>
       </c>
       <c r="C11" t="n">
-        <v>44.941605</v>
+        <v>12.9972363113479</v>
       </c>
       <c r="D11" t="n">
-        <v>12.9972363113479</v>
+        <v>468.395521654458</v>
       </c>
       <c r="E11" t="n">
-        <v>468.395521654458</v>
+        <v>75.68681660962361</v>
       </c>
       <c r="F11" t="n">
-        <v>11.9478354691139</v>
+        <v>13.9036865990995</v>
       </c>
       <c r="G11" t="n">
-        <v>75.68681660962361</v>
+        <v>27.3258283775917</v>
       </c>
       <c r="H11" t="n">
-        <v>13.9036865990995</v>
+        <v>4.0094359104519</v>
       </c>
       <c r="I11" t="n">
-        <v>27.3258283775917</v>
-      </c>
-      <c r="J11" t="n">
-        <v>4.0094359104519</v>
-      </c>
-      <c r="K11" t="n">
-        <v>12.2916666666667</v>
-      </c>
-      <c r="L11" t="n">
         <v>25.677316683955</v>
-      </c>
-      <c r="M11" t="n">
-        <v>54.6451291831448</v>
-      </c>
-      <c r="N11" t="n">
-        <v>7.624</v>
       </c>
     </row>
     <row r="12">
@@ -975,40 +800,25 @@
         <v>0.290495460210207</v>
       </c>
       <c r="C12" t="n">
-        <v>47.1864141666667</v>
+        <v>12.5583796339108</v>
       </c>
       <c r="D12" t="n">
-        <v>12.5583796339108</v>
+        <v>485.440139204171</v>
       </c>
       <c r="E12" t="n">
-        <v>485.440139204171</v>
+        <v>75.90830731653929</v>
       </c>
       <c r="F12" t="n">
-        <v>11.7614498890899</v>
+        <v>13.4348751195257</v>
       </c>
       <c r="G12" t="n">
-        <v>75.90830731653929</v>
+        <v>26.4877773440307</v>
       </c>
       <c r="H12" t="n">
-        <v>13.4348751195257</v>
+        <v>3.77929312235637</v>
       </c>
       <c r="I12" t="n">
-        <v>26.4877773440307</v>
-      </c>
-      <c r="J12" t="n">
-        <v>3.77929312235637</v>
-      </c>
-      <c r="K12" t="n">
-        <v>12.0833333333333</v>
-      </c>
-      <c r="L12" t="n">
         <v>29.9078889827325</v>
-      </c>
-      <c r="M12" t="n">
-        <v>57.7390677682671</v>
-      </c>
-      <c r="N12" t="n">
-        <v>7.653</v>
       </c>
     </row>
     <row r="13">
@@ -1021,40 +831,25 @@
         <v>1.37093793900847</v>
       </c>
       <c r="C13" t="n">
-        <v>48.6103191666667</v>
+        <v>14.2643839243147</v>
       </c>
       <c r="D13" t="n">
-        <v>14.2643839243147</v>
+        <v>514.939140318756</v>
       </c>
       <c r="E13" t="n">
-        <v>514.939140318756</v>
+        <v>74.3437418253318</v>
       </c>
       <c r="F13" t="n">
-        <v>11.3140950692424</v>
+        <v>15.2442790107467</v>
       </c>
       <c r="G13" t="n">
-        <v>74.3437418253318</v>
+        <v>27.6606541607882</v>
       </c>
       <c r="H13" t="n">
-        <v>15.2442790107467</v>
+        <v>4.29715203929563</v>
       </c>
       <c r="I13" t="n">
-        <v>27.6606541607882</v>
-      </c>
-      <c r="J13" t="n">
-        <v>4.29715203929563</v>
-      </c>
-      <c r="K13" t="n">
-        <v>11.9166666666667</v>
-      </c>
-      <c r="L13" t="n">
         <v>30.2513001207186</v>
-      </c>
-      <c r="M13" t="n">
-        <v>62.6195245160236</v>
-      </c>
-      <c r="N13" t="n">
-        <v>7.753</v>
       </c>
     </row>
     <row r="14">
@@ -1067,40 +862,25 @@
         <v>1.44355773291234</v>
       </c>
       <c r="C14" t="n">
-        <v>46.5832841666667</v>
+        <v>14.9479138581734</v>
       </c>
       <c r="D14" t="n">
-        <v>14.9479138581734</v>
+        <v>607.700687237318</v>
       </c>
       <c r="E14" t="n">
-        <v>607.700687237318</v>
+        <v>72.37996752245191</v>
       </c>
       <c r="F14" t="n">
-        <v>10.8762099129119</v>
+        <v>15.6445222747346</v>
       </c>
       <c r="G14" t="n">
-        <v>72.37996752245191</v>
+        <v>27.4741071211988</v>
       </c>
       <c r="H14" t="n">
-        <v>15.6445222747346</v>
+        <v>3.80585899528851</v>
       </c>
       <c r="I14" t="n">
-        <v>27.4741071211988</v>
-      </c>
-      <c r="J14" t="n">
-        <v>3.80585899528851</v>
-      </c>
-      <c r="K14" t="n">
-        <v>11.4583333333333</v>
-      </c>
-      <c r="L14" t="n">
         <v>30.8396999424416</v>
-      </c>
-      <c r="M14" t="n">
-        <v>63.1792536038838</v>
-      </c>
-      <c r="N14" t="n">
-        <v>7.68</v>
       </c>
     </row>
     <row r="15">
@@ -1113,40 +893,25 @@
         <v>0.110018010197153</v>
       </c>
       <c r="C15" t="n">
-        <v>45.3164666666666</v>
+        <v>17.8591249630479</v>
       </c>
       <c r="D15" t="n">
-        <v>17.8591249630479</v>
+        <v>709.152728830775</v>
       </c>
       <c r="E15" t="n">
-        <v>709.152728830775</v>
+        <v>68.7562502876863</v>
       </c>
       <c r="F15" t="n">
-        <v>10.4047023481415</v>
+        <v>19.6446890963991</v>
       </c>
       <c r="G15" t="n">
-        <v>68.7562502876863</v>
+        <v>29.219106305293</v>
       </c>
       <c r="H15" t="n">
-        <v>19.6446890963991</v>
+        <v>3.76725173477515</v>
       </c>
       <c r="I15" t="n">
-        <v>29.219106305293</v>
-      </c>
-      <c r="J15" t="n">
-        <v>3.76725173477515</v>
-      </c>
-      <c r="K15" t="n">
-        <v>10.9166666666667</v>
-      </c>
-      <c r="L15" t="n">
         <v>35.0964917017773</v>
-      </c>
-      <c r="M15" t="n">
-        <v>64.6357080581913</v>
-      </c>
-      <c r="N15" t="n">
-        <v>7.625</v>
       </c>
     </row>
     <row r="16">
@@ -1159,40 +924,25 @@
         <v>-1.25350400207393</v>
       </c>
       <c r="C16" t="n">
-        <v>44.099975</v>
+        <v>19.6052466948335</v>
       </c>
       <c r="D16" t="n">
-        <v>19.6052466948335</v>
+        <v>820.383763511445</v>
       </c>
       <c r="E16" t="n">
-        <v>820.383763511445</v>
+        <v>67.744870132719</v>
       </c>
       <c r="F16" t="n">
-        <v>10.3661401972455</v>
+        <v>22.3964229200356</v>
       </c>
       <c r="G16" t="n">
-        <v>67.744870132719</v>
+        <v>29.5337641914637</v>
       </c>
       <c r="H16" t="n">
-        <v>22.3964229200356</v>
+        <v>4.24634362031922</v>
       </c>
       <c r="I16" t="n">
-        <v>29.5337641914637</v>
-      </c>
-      <c r="J16" t="n">
-        <v>4.24634362031922</v>
-      </c>
-      <c r="K16" t="n">
-        <v>10.75</v>
-      </c>
-      <c r="L16" t="n">
         <v>37.4282640165983</v>
-      </c>
-      <c r="M16" t="n">
-        <v>65.5481218951747</v>
-      </c>
-      <c r="N16" t="n">
-        <v>7.552</v>
       </c>
     </row>
     <row r="17">
@@ -1205,40 +955,25 @@
         <v>-0.988988302952292</v>
       </c>
       <c r="C17" t="n">
-        <v>45.3070083333333</v>
+        <v>21.2679414221966</v>
       </c>
       <c r="D17" t="n">
-        <v>21.2679414221966</v>
+        <v>940.2598887877209</v>
       </c>
       <c r="E17" t="n">
-        <v>940.2598887877209</v>
+        <v>65.9124158733367</v>
       </c>
       <c r="F17" t="n">
-        <v>9.80247046783494</v>
+        <v>24.4565390770687</v>
       </c>
       <c r="G17" t="n">
-        <v>65.9124158733367</v>
+        <v>30.9272399435883</v>
       </c>
       <c r="H17" t="n">
-        <v>24.4565390770687</v>
+        <v>5.79652337561634</v>
       </c>
       <c r="I17" t="n">
-        <v>30.9272399435883</v>
-      </c>
-      <c r="J17" t="n">
-        <v>5.79652337561634</v>
-      </c>
-      <c r="K17" t="n">
-        <v>11.1875</v>
-      </c>
-      <c r="L17" t="n">
         <v>38.9985063717532</v>
-      </c>
-      <c r="M17" t="n">
-        <v>68.0630217874844</v>
-      </c>
-      <c r="N17" t="n">
-        <v>7.552</v>
       </c>
     </row>
     <row r="18">
@@ -1251,40 +986,25 @@
         <v>-0.66371764877261</v>
       </c>
       <c r="C18" t="n">
-        <v>41.3485333333333</v>
+        <v>20.7996997489032</v>
       </c>
       <c r="D18" t="n">
-        <v>20.7996997489032</v>
+        <v>1216.73643883496</v>
       </c>
       <c r="E18" t="n">
-        <v>1216.73643883496</v>
+        <v>65.62262680394591</v>
       </c>
       <c r="F18" t="n">
-        <v>9.862115728426421</v>
+        <v>24.8865689304448</v>
       </c>
       <c r="G18" t="n">
-        <v>65.62262680394591</v>
+        <v>30.9032382510869</v>
       </c>
       <c r="H18" t="n">
-        <v>24.8865689304448</v>
+        <v>6.37288135593231</v>
       </c>
       <c r="I18" t="n">
-        <v>30.9032382510869</v>
-      </c>
-      <c r="J18" t="n">
-        <v>6.37288135593231</v>
-      </c>
-      <c r="K18" t="n">
-        <v>13.0208333333333</v>
-      </c>
-      <c r="L18" t="n">
         <v>41.9507982267334</v>
-      </c>
-      <c r="M18" t="n">
-        <v>72.2804239219053</v>
-      </c>
-      <c r="N18" t="n">
-        <v>7.561</v>
       </c>
     </row>
     <row r="19">
@@ -1297,40 +1017,25 @@
         <v>-2.58337749259838</v>
       </c>
       <c r="C19" t="n">
-        <v>43.5051833333333</v>
+        <v>24.0973572601391</v>
       </c>
       <c r="D19" t="n">
-        <v>24.0973572601391</v>
+        <v>1198.89513900592</v>
       </c>
       <c r="E19" t="n">
-        <v>1198.89513900592</v>
+        <v>67.2152971379759</v>
       </c>
       <c r="F19" t="n">
-        <v>10.5384811563533</v>
+        <v>29.2708631790835</v>
       </c>
       <c r="G19" t="n">
-        <v>67.2152971379759</v>
+        <v>31.1367192409548</v>
       </c>
       <c r="H19" t="n">
-        <v>29.2708631790835</v>
+        <v>8.349267049075809</v>
       </c>
       <c r="I19" t="n">
-        <v>31.1367192409548</v>
-      </c>
-      <c r="J19" t="n">
-        <v>8.349267049075809</v>
-      </c>
-      <c r="K19" t="n">
-        <v>13.3125</v>
-      </c>
-      <c r="L19" t="n">
         <v>38.4224196528192</v>
-      </c>
-      <c r="M19" t="n">
-        <v>77.3729561105341</v>
-      </c>
-      <c r="N19" t="n">
-        <v>7.656</v>
       </c>
     </row>
     <row r="20">
@@ -1343,40 +1048,25 @@
         <v>-1.95146209111802</v>
       </c>
       <c r="C20" t="n">
-        <v>48.4052666666666</v>
+        <v>20.4005193743564</v>
       </c>
       <c r="D20" t="n">
-        <v>20.4005193743564</v>
+        <v>1341.8880169949</v>
       </c>
       <c r="E20" t="n">
-        <v>1341.8880169949</v>
+        <v>67.4195558848204</v>
       </c>
       <c r="F20" t="n">
-        <v>11.459667419691</v>
+        <v>25.8723502685274</v>
       </c>
       <c r="G20" t="n">
-        <v>67.4195558848204</v>
+        <v>31.1213721116744</v>
       </c>
       <c r="H20" t="n">
-        <v>25.8723502685274</v>
+        <v>10.8823529411764</v>
       </c>
       <c r="I20" t="n">
-        <v>31.1213721116744</v>
-      </c>
-      <c r="J20" t="n">
-        <v>10.8823529411764</v>
-      </c>
-      <c r="K20" t="n">
-        <v>12.1875</v>
-      </c>
-      <c r="L20" t="n">
         <v>39.2567917551336</v>
-      </c>
-      <c r="M20" t="n">
-        <v>79.0751963448471</v>
-      </c>
-      <c r="N20" t="n">
-        <v>7.664</v>
       </c>
     </row>
     <row r="21">
@@ -1389,40 +1079,25 @@
         <v>-3.25348368945179</v>
       </c>
       <c r="C21" t="n">
-        <v>45.7258121212121</v>
+        <v>22.4009332487945</v>
       </c>
       <c r="D21" t="n">
-        <v>22.4009332487945</v>
+        <v>1675.61551948496</v>
       </c>
       <c r="E21" t="n">
-        <v>1675.61551948496</v>
+        <v>65.7324656294299</v>
       </c>
       <c r="F21" t="n">
-        <v>11.0076078674499</v>
+        <v>26.8542732486216</v>
       </c>
       <c r="G21" t="n">
-        <v>65.7324656294299</v>
+        <v>30.7250782285817</v>
       </c>
       <c r="H21" t="n">
-        <v>26.8542732486216</v>
+        <v>11.9893899204244</v>
       </c>
       <c r="I21" t="n">
-        <v>30.7250782285817</v>
-      </c>
-      <c r="J21" t="n">
-        <v>11.9893899204244</v>
-      </c>
-      <c r="K21" t="n">
-        <v>8.333349999999999</v>
-      </c>
-      <c r="L21" t="n">
         <v>39.7856241847736</v>
-      </c>
-      <c r="M21" t="n">
-        <v>77.67995244357</v>
-      </c>
-      <c r="N21" t="n">
-        <v>7.652</v>
       </c>
     </row>
     <row r="22">
@@ -1435,40 +1110,25 @@
         <v>-3.42928468606061</v>
       </c>
       <c r="C22" t="n">
-        <v>46.6704666666667</v>
+        <v>24.5404113195713</v>
       </c>
       <c r="D22" t="n">
-        <v>24.5404113195713</v>
+        <v>1823.05182989455</v>
       </c>
       <c r="E22" t="n">
-        <v>1823.05182989455</v>
+        <v>67.29168016994301</v>
       </c>
       <c r="F22" t="n">
-        <v>11.0844615855594</v>
+        <v>31.0834686939585</v>
       </c>
       <c r="G22" t="n">
-        <v>67.29168016994301</v>
+        <v>30.1616797630407</v>
       </c>
       <c r="H22" t="n">
-        <v>31.0834686939585</v>
+        <v>8.911793364833709</v>
       </c>
       <c r="I22" t="n">
-        <v>30.1616797630407</v>
-      </c>
-      <c r="J22" t="n">
-        <v>8.911793364833709</v>
-      </c>
-      <c r="K22" t="n">
-        <v>10.1666666666667</v>
-      </c>
-      <c r="L22" t="n">
         <v>39.590421855219</v>
-      </c>
-      <c r="M22" t="n">
-        <v>78.8373112865613</v>
-      </c>
-      <c r="N22" t="n">
-        <v>7.616</v>
       </c>
     </row>
     <row r="23">
@@ -1481,40 +1141,25 @@
         <v>-5.00488971805303</v>
       </c>
       <c r="C23" t="n">
-        <v>53.4372333333333</v>
+        <v>24.534430661418</v>
       </c>
       <c r="D23" t="n">
-        <v>24.534430661418</v>
+        <v>1827.63759041041</v>
       </c>
       <c r="E23" t="n">
-        <v>1827.63759041041</v>
+        <v>67.1448100211522</v>
       </c>
       <c r="F23" t="n">
-        <v>10.6838562318127</v>
+        <v>31.2592910673332</v>
       </c>
       <c r="G23" t="n">
-        <v>67.1448100211522</v>
+        <v>29.3985276965289</v>
       </c>
       <c r="H23" t="n">
-        <v>31.2592910673332</v>
+        <v>9.47899691419801</v>
       </c>
       <c r="I23" t="n">
-        <v>29.3985276965289</v>
-      </c>
-      <c r="J23" t="n">
-        <v>9.47899691419801</v>
-      </c>
-      <c r="K23" t="n">
-        <v>10.6041666666667</v>
-      </c>
-      <c r="L23" t="n">
         <v>38.3474156730403</v>
-      </c>
-      <c r="M23" t="n">
-        <v>76.91318852057491</v>
-      </c>
-      <c r="N23" t="n">
-        <v>7.666</v>
       </c>
     </row>
     <row r="24">
@@ -1527,40 +1172,25 @@
         <v>-2.64566711733892</v>
       </c>
       <c r="C24" t="n">
-        <v>58.5978454166667</v>
+        <v>25.430861300519</v>
       </c>
       <c r="D24" t="n">
-        <v>25.430861300519</v>
+        <v>1856.72150762158</v>
       </c>
       <c r="E24" t="n">
-        <v>1856.72150762158</v>
+        <v>67.94092623280019</v>
       </c>
       <c r="F24" t="n">
-        <v>10.2951601419598</v>
+        <v>28.4132706461587</v>
       </c>
       <c r="G24" t="n">
-        <v>67.94092623280019</v>
+        <v>28.4048995600246</v>
       </c>
       <c r="H24" t="n">
-        <v>28.4132706461587</v>
+        <v>10.0178784746102</v>
       </c>
       <c r="I24" t="n">
-        <v>28.4048995600246</v>
-      </c>
-      <c r="J24" t="n">
-        <v>10.0178784746102</v>
-      </c>
-      <c r="K24" t="n">
-        <v>10.2916666666667</v>
-      </c>
-      <c r="L24" t="n">
         <v>34.0231978997548</v>
-      </c>
-      <c r="M24" t="n">
-        <v>78.1821717320597</v>
-      </c>
-      <c r="N24" t="n">
-        <v>7.711</v>
       </c>
     </row>
     <row r="25">
@@ -1573,40 +1203,25 @@
         <v>-1.33950896483453</v>
       </c>
       <c r="C25" t="n">
-        <v>61.0295144607843</v>
+        <v>22.9679630081172</v>
       </c>
       <c r="D25" t="n">
-        <v>22.9679630081172</v>
+        <v>2039.12647915452</v>
       </c>
       <c r="E25" t="n">
-        <v>2039.12647915452</v>
+        <v>68.56857390943171</v>
       </c>
       <c r="F25" t="n">
-        <v>10.4408568081213</v>
+        <v>25.9542227389497</v>
       </c>
       <c r="G25" t="n">
-        <v>68.56857390943171</v>
+        <v>27.6564012026443</v>
       </c>
       <c r="H25" t="n">
-        <v>25.9542227389497</v>
+        <v>6.66565671867899</v>
       </c>
       <c r="I25" t="n">
-        <v>27.6564012026443</v>
-      </c>
-      <c r="J25" t="n">
-        <v>6.66565671867899</v>
-      </c>
-      <c r="K25" t="n">
-        <v>10.25</v>
-      </c>
-      <c r="L25" t="n">
         <v>34.2678056268836</v>
-      </c>
-      <c r="M25" t="n">
-        <v>77.8993537588766</v>
-      </c>
-      <c r="N25" t="n">
-        <v>7.674</v>
       </c>
     </row>
     <row r="26">
@@ -1619,40 +1234,25 @@
         <v>-1.06754907167965</v>
       </c>
       <c r="C26" t="n">
-        <v>64.1519444632786</v>
+        <v>19.8131891564045</v>
       </c>
       <c r="D26" t="n">
-        <v>19.8131891564045</v>
+        <v>2103.58836004494</v>
       </c>
       <c r="E26" t="n">
-        <v>2103.58836004494</v>
+        <v>69.43557178699319</v>
       </c>
       <c r="F26" t="n">
-        <v>10.4282907091862</v>
+        <v>22.1097247094602</v>
       </c>
       <c r="G26" t="n">
-        <v>69.43557178699319</v>
+        <v>27.34739147794</v>
       </c>
       <c r="H26" t="n">
-        <v>22.1097247094602</v>
+        <v>4.90697344127256</v>
       </c>
       <c r="I26" t="n">
-        <v>27.34739147794</v>
-      </c>
-      <c r="J26" t="n">
-        <v>4.90697344127256</v>
-      </c>
-      <c r="K26" t="n">
-        <v>10.0083333333333</v>
-      </c>
-      <c r="L26" t="n">
         <v>32.1167301358276</v>
-      </c>
-      <c r="M26" t="n">
-        <v>78.0119105841633</v>
-      </c>
-      <c r="N26" t="n">
-        <v>7.631</v>
       </c>
     </row>
     <row r="27">
@@ -1665,40 +1265,25 @@
         <v>-0.52788060603752</v>
       </c>
       <c r="C27" t="n">
-        <v>67.1953128073894</v>
+        <v>19.1582349105946</v>
       </c>
       <c r="D27" t="n">
-        <v>19.1582349105946</v>
+        <v>2294.79688566316</v>
       </c>
       <c r="E27" t="n">
-        <v>2294.79688566316</v>
+        <v>69.6038293075294</v>
       </c>
       <c r="F27" t="n">
-        <v>10.3085480747222</v>
+        <v>20.9242508026814</v>
       </c>
       <c r="G27" t="n">
-        <v>69.6038293075294</v>
+        <v>26.6189999399789</v>
       </c>
       <c r="H27" t="n">
-        <v>20.9242508026814</v>
+        <v>4.94821634062141</v>
       </c>
       <c r="I27" t="n">
-        <v>26.6189999399789</v>
-      </c>
-      <c r="J27" t="n">
-        <v>4.94821634062141</v>
-      </c>
-      <c r="K27" t="n">
-        <v>9.672499999999999</v>
-      </c>
-      <c r="L27" t="n">
         <v>30.172690580036</v>
-      </c>
-      <c r="M27" t="n">
-        <v>74.54926535196169</v>
-      </c>
-      <c r="N27" t="n">
-        <v>7.601</v>
       </c>
     </row>
     <row r="28">
@@ -1711,40 +1296,25 @@
         <v>-1.43948820320989</v>
       </c>
       <c r="C28" t="n">
-        <v>65.12156864506591</v>
+        <v>18.7917648392982</v>
       </c>
       <c r="D28" t="n">
-        <v>18.7917648392982</v>
+        <v>2651.47426275545</v>
       </c>
       <c r="E28" t="n">
-        <v>2651.47426275545</v>
+        <v>69.4923486310466</v>
       </c>
       <c r="F28" t="n">
-        <v>10.7671989547856</v>
+        <v>21.9507321152243</v>
       </c>
       <c r="G28" t="n">
-        <v>69.4923486310466</v>
+        <v>26.5000166464804</v>
       </c>
       <c r="H28" t="n">
-        <v>21.9507321152243</v>
+        <v>3.32817337461298</v>
       </c>
       <c r="I28" t="n">
-        <v>26.5000166464804</v>
-      </c>
-      <c r="J28" t="n">
-        <v>3.32817337461298</v>
-      </c>
-      <c r="K28" t="n">
-        <v>9.508333333333329</v>
-      </c>
-      <c r="L28" t="n">
         <v>30.9821728344733</v>
-      </c>
-      <c r="M28" t="n">
-        <v>74.1441893624702</v>
-      </c>
-      <c r="N28" t="n">
-        <v>7.618</v>
       </c>
     </row>
     <row r="29">
@@ -1757,40 +1327,25 @@
         <v>-2.42697545810527</v>
       </c>
       <c r="C29" t="n">
-        <v>68.38946709354219</v>
+        <v>19.9278285988562</v>
       </c>
       <c r="D29" t="n">
-        <v>19.9278285988562</v>
+        <v>2702.92964164874</v>
       </c>
       <c r="E29" t="n">
-        <v>2702.92964164874</v>
+        <v>70.1115413382452</v>
       </c>
       <c r="F29" t="n">
-        <v>10.8232185258548</v>
+        <v>23.6891407335327</v>
       </c>
       <c r="G29" t="n">
-        <v>70.1115413382452</v>
+        <v>26.4120919013735</v>
       </c>
       <c r="H29" t="n">
-        <v>23.6891407335327</v>
+        <v>3.9388264669163</v>
       </c>
       <c r="I29" t="n">
-        <v>26.4120919013735</v>
-      </c>
-      <c r="J29" t="n">
-        <v>3.9388264669163</v>
-      </c>
-      <c r="K29" t="n">
-        <v>9.454166666666669</v>
-      </c>
-      <c r="L29" t="n">
         <v>32.3432182154485</v>
-      </c>
-      <c r="M29" t="n">
-        <v>74.09782460471099</v>
-      </c>
-      <c r="N29" t="n">
-        <v>7.652</v>
       </c>
     </row>
     <row r="30">
@@ -1803,40 +1358,25 @@
         <v>-1.04961203910072</v>
       </c>
       <c r="C30" t="n">
-        <v>70.42034053595511</v>
+        <v>18.664264897257</v>
       </c>
       <c r="D30" t="n">
-        <v>18.664264897257</v>
+        <v>2835.60625655819</v>
       </c>
       <c r="E30" t="n">
-        <v>2835.60625655819</v>
+        <v>71.9139631514218</v>
       </c>
       <c r="F30" t="n">
-        <v>11.0026755133718</v>
+        <v>21.2411386333872</v>
       </c>
       <c r="G30" t="n">
-        <v>71.9139631514218</v>
+        <v>24.5914753075066</v>
       </c>
       <c r="H30" t="n">
-        <v>21.2411386333872</v>
+        <v>3.72950573539129</v>
       </c>
       <c r="I30" t="n">
-        <v>24.5914753075066</v>
-      </c>
-      <c r="J30" t="n">
-        <v>3.72950573539129</v>
-      </c>
-      <c r="K30" t="n">
-        <v>9.46625</v>
-      </c>
-      <c r="L30" t="n">
         <v>30.0961975685688</v>
-      </c>
-      <c r="M30" t="n">
-        <v>76.98188096813</v>
-      </c>
-      <c r="N30" t="n">
-        <v>6.51</v>
       </c>
     </row>
     <row r="31">
@@ -1849,40 +1389,25 @@
         <v>1.22362111042791</v>
       </c>
       <c r="C31" t="n">
-        <v>74.09956688360521</v>
+        <v>18.6824769296756</v>
       </c>
       <c r="D31" t="n">
-        <v>18.6824769296756</v>
+        <v>2674.85157858727</v>
       </c>
       <c r="E31" t="n">
-        <v>2674.85157858727</v>
+        <v>72.71058112091229</v>
       </c>
       <c r="F31" t="n">
-        <v>11.6124524106018</v>
+        <v>19.0756283996012</v>
       </c>
       <c r="G31" t="n">
-        <v>72.71058112091229</v>
+        <v>25.1229058078344</v>
       </c>
       <c r="H31" t="n">
-        <v>19.0756283996012</v>
+        <v>6.62343677628535</v>
       </c>
       <c r="I31" t="n">
-        <v>25.1229058078344</v>
-      </c>
-      <c r="J31" t="n">
-        <v>6.62343677628535</v>
-      </c>
-      <c r="K31" t="n">
-        <v>9.15</v>
-      </c>
-      <c r="L31" t="n">
         <v>28.9223840080659</v>
-      </c>
-      <c r="M31" t="n">
-        <v>87.6766726830318</v>
-      </c>
-      <c r="N31" t="n">
-        <v>7.859</v>
       </c>
     </row>
     <row r="32">
@@ -1895,40 +1420,118 @@
         <v>-1.05524166809383</v>
       </c>
       <c r="C32" t="n">
-        <v>73.91801281543511</v>
+        <v>21.3991583305515</v>
       </c>
       <c r="D32" t="n">
-        <v>21.3991583305515</v>
+        <v>3167.27062326047</v>
       </c>
       <c r="E32" t="n">
-        <v>3167.27062326047</v>
+        <v>71.4267578736418</v>
       </c>
       <c r="F32" t="n">
-        <v>10.4763782400684</v>
+        <v>24.0239304534931</v>
       </c>
       <c r="G32" t="n">
-        <v>71.4267578736418</v>
+        <v>26.466523606501</v>
       </c>
       <c r="H32" t="n">
-        <v>24.0239304534931</v>
+        <v>5.13140747176369</v>
       </c>
       <c r="I32" t="n">
-        <v>26.466523606501</v>
-      </c>
-      <c r="J32" t="n">
-        <v>5.13140747176369</v>
-      </c>
-      <c r="K32" t="n">
-        <v>8.698333333333331</v>
-      </c>
-      <c r="L32" t="n">
         <v>32.1158221755014</v>
       </c>
-      <c r="M32" t="n">
-        <v>82.1020348312414</v>
-      </c>
-      <c r="N32" t="n">
-        <v>6.38</v>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>-2.36247481487452</v>
+      </c>
+      <c r="C33" t="n">
+        <v>23.2515412045298</v>
+      </c>
+      <c r="D33" t="n">
+        <v>3346.10728773093</v>
+      </c>
+      <c r="E33" t="n">
+        <v>71.7186722536094</v>
+      </c>
+      <c r="F33" t="n">
+        <v>26.8237289453584</v>
+      </c>
+      <c r="G33" t="n">
+        <v>25.3845195629461</v>
+      </c>
+      <c r="H33" t="n">
+        <v>6.69903414079852</v>
+      </c>
+      <c r="I33" t="n">
+        <v>33.6192585388984</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>-0.878449448896405</v>
+      </c>
+      <c r="C34" t="n">
+        <v>21.4486977833541</v>
+      </c>
+      <c r="D34" t="n">
+        <v>3638.48909603386</v>
+      </c>
+      <c r="E34" t="n">
+        <v>70.49351104436801</v>
+      </c>
+      <c r="F34" t="n">
+        <v>23.544144504402</v>
+      </c>
+      <c r="G34" t="n">
+        <v>25.302936496264</v>
+      </c>
+      <c r="H34" t="n">
+        <v>5.64914318907925</v>
+      </c>
+      <c r="I34" t="n">
+        <v>33.3623103638844</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>-0.828801355740078</v>
+      </c>
+      <c r="C35" t="n">
+        <v>21.1781223210845</v>
+      </c>
+      <c r="D35" t="n">
+        <v>3912.68616858221</v>
+      </c>
+      <c r="E35" t="n">
+        <v>71.63128590118841</v>
+      </c>
+      <c r="F35" t="n">
+        <v>23.4929703141577</v>
+      </c>
+      <c r="G35" t="n">
+        <v>24.4649305051595</v>
+      </c>
+      <c r="H35" t="n">
+        <v>4.95303550973656</v>
+      </c>
+      <c r="I35" t="n">
+        <v>32.6109099957867</v>
       </c>
     </row>
   </sheetData>

</xml_diff>